<commit_message>
teame profile view & edit
</commit_message>
<xml_diff>
--- a/documentation/timing/Time Sheet1.xlsx
+++ b/documentation/timing/Time Sheet1.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -347,8 +347,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G16" totalsRowShown="0">
-  <autoFilter ref="B7:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G17" totalsRowShown="0">
+  <autoFilter ref="B7:G17"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date(s)" dataCellStyle="Date"/>
     <tableColumn id="2" name="Time In" dataCellStyle="Time"/>
@@ -635,10 +635,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:L16"/>
+  <dimension ref="B1:L17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -716,19 +716,19 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>26.25</v>
+        <v>42.55</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
-        <v>26.25</v>
+        <v>40</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
-        <v>0</v>
+        <v>2.5499999999999972</v>
       </c>
       <c r="J6" s="13">
         <f ca="1">NOW()</f>
-        <v>42895.054697453706</v>
+        <v>42895.453253587963</v>
       </c>
       <c r="L6" s="13"/>
     </row>
@@ -942,6 +942,27 @@
       <c r="G16" s="5">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>0.80000000000000249</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="4">
+        <v>42895</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="6">
+        <v>9.5833333333333298E-2</v>
+      </c>
+      <c r="G17" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>16.299999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create action of school panel
</commit_message>
<xml_diff>
--- a/documentation/timing/Time Sheet1.xlsx
+++ b/documentation/timing/Time Sheet1.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -347,8 +347,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G22" totalsRowShown="0">
-  <autoFilter ref="B7:G22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G25" totalsRowShown="0">
+  <autoFilter ref="B7:G25"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date(s)" dataCellStyle="Date"/>
     <tableColumn id="2" name="Time In" dataCellStyle="Time"/>
@@ -635,10 +635,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:L22"/>
+  <dimension ref="B1:L25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -716,7 +716,7 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>72.766666666666666</v>
+        <v>89.266666666666666</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -724,11 +724,11 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
-        <v>32.766666666666666</v>
+        <v>49.266666666666666</v>
       </c>
       <c r="J6" s="13">
         <f ca="1">NOW()</f>
-        <v>42900.216085879627</v>
+        <v>42902.811343055553</v>
       </c>
       <c r="L6" s="13"/>
     </row>
@@ -1068,6 +1068,69 @@
       <c r="G22" s="5">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>5.166666666666667</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="4">
+        <v>42900</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="G23" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="4">
+        <v>42901</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G24" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="4">
+        <v>42902</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G25" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>3.9999999999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set access an cntroller admin panels
</commit_message>
<xml_diff>
--- a/documentation/timing/Time Sheet1.xlsx
+++ b/documentation/timing/Time Sheet1.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -223,7 +223,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -264,6 +264,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -347,8 +350,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G25" totalsRowShown="0">
-  <autoFilter ref="B7:G25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G27" totalsRowShown="0">
+  <autoFilter ref="B7:G27"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date(s)" dataCellStyle="Date"/>
     <tableColumn id="2" name="Time In" dataCellStyle="Time"/>
@@ -635,10 +638,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:L25"/>
+  <dimension ref="B1:L27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -716,7 +719,7 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>89.266666666666666</v>
+        <v>100.21666666666665</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -724,11 +727,11 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
-        <v>49.266666666666666</v>
+        <v>60.216666666666654</v>
       </c>
       <c r="J6" s="13">
         <f ca="1">NOW()</f>
-        <v>42902.811343055553</v>
+        <v>42905.45656053241</v>
       </c>
       <c r="L6" s="13"/>
     </row>
@@ -944,7 +947,7 @@
         <v>0.80000000000000249</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="4">
         <v>42895</v>
       </c>
@@ -965,7 +968,7 @@
         <v>11.766666666666666</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4">
         <v>42896</v>
       </c>
@@ -986,7 +989,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="4">
         <v>42897</v>
       </c>
@@ -1007,7 +1010,7 @@
         <v>9.4999999999999982</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="4">
         <v>42898</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="4">
         <v>42899</v>
       </c>
@@ -1049,7 +1052,7 @@
         <v>4.9833333333333343</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="4">
         <v>42900</v>
       </c>
@@ -1070,7 +1073,7 @@
         <v>5.166666666666667</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="4">
         <v>42900</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="4">
         <v>42901</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="4">
         <v>42902</v>
       </c>
@@ -1131,6 +1134,51 @@
       <c r="G25" s="5">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>3.9999999999999991</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="4">
+        <v>42904</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.9506944444444444</v>
+      </c>
+      <c r="G26" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0.8999999999999968</v>
+      </c>
+      <c r="J26" s="14">
+        <v>0.9506944444444444</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="4">
+        <v>42905</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.45624999999999999</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="G27" s="5">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>10.050000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>